<commit_message>
Cambios cuentas por pagar
</commit_message>
<xml_diff>
--- a/Ppgz/Ppgz.Web/App_Data/plantilladevoluciones.xlsx
+++ b/Ppgz/Ppgz.Web/App_Data/plantilladevoluciones.xlsx
@@ -42,9 +42,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>CATNIDAD</t>
-  </si>
-  <si>
     <t>TOTAL PARES DEVUELTOS:</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>DEVOLUCIONES</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
   </si>
 </sst>
 </file>
@@ -248,6 +248,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -257,23 +269,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D909"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,18 +641,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>12</v>
+      <c r="A1" s="22" t="s">
+        <v>11</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -676,9 +676,9 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -686,19 +686,19 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="26"/>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
@@ -717,7 +717,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>